<commit_message>
Lots of changes, README.md created
</commit_message>
<xml_diff>
--- a/Data/Raw/resumen_variables_tfm.xlsx
+++ b/Data/Raw/resumen_variables_tfm.xlsx
@@ -1127,11 +1127,11 @@
   </sheetPr>
   <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G131" activeCellId="0" sqref="G131"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="95.86"/>
@@ -1227,7 +1227,6 @@
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">

</xml_diff>